<commit_message>
Graba Coordenadas en No Entregados y Rechazados
</commit_message>
<xml_diff>
--- a/LO QUE CAMBIA EN ENVIOS Y PARADAS.xlsx
+++ b/LO QUE CAMBIA EN ENVIOS Y PARADAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\fleetdeliveryapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41B485C-1F71-483C-842B-FEEB39C29D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F903DE9-826C-4468-97C0-C5C98CB88C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9CDC810F-665F-4E82-997D-B77DDCCC3EAE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="180">
   <si>
     <t>ANTES DE GRABAR</t>
   </si>
@@ -563,6 +563,18 @@
   </si>
   <si>
     <t>SELECT ID, ESTADO, FechaEntregaCliente, FechaUltimaActualizacion, UltimoIdMotivo, UltimaNotaFletero, UrlDNI,LATITUD2,LONGITUD2</t>
+  </si>
+  <si>
+    <t>SELECT IdEnvio,ID, Estado, Fecha, Hora, IdMotivo, NotaChofer, Secuencia</t>
+  </si>
+  <si>
+    <t>WHERE  (IdRuta = 2425)</t>
+  </si>
+  <si>
+    <t>ORDER BY IdEnvio</t>
+  </si>
+  <si>
+    <t>WHERE  (NroRuta = 2425)</t>
   </si>
 </sst>
 </file>
@@ -678,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -710,6 +722,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED9E5AD-1D27-4A0E-AF14-E382028640F8}">
   <dimension ref="A1:BU60"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3554,10 +3567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34CE9C5-308F-4DC4-BC67-C26EED04CDA8}">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3894,6 +3907,52 @@
         <v>170</v>
       </c>
     </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="29" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="29"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="29"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>